<commit_message>
Update homepage for cleanliness
</commit_message>
<xml_diff>
--- a/src/static/Shufu no tomo Metadata.xlsx
+++ b/src/static/Shufu no tomo Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theodoreliu/visual-tokyo/src/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4310B832-0A1C-B24C-AD25-1BF53FAE37B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82D6904-EB56-7943-9BE7-A3C4725E2A1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="298">
   <si>
     <t>Folder name</t>
   </si>
@@ -458,18 +458,6 @@
   </si>
   <si>
     <t>clothing</t>
-  </si>
-  <si>
-    <t>shufu.28.001.jpg</t>
-  </si>
-  <si>
-    <t>shufu.28.002.jpg</t>
-  </si>
-  <si>
-    <t>Azumabashi</t>
-  </si>
-  <si>
-    <t>Azuma Bridge</t>
   </si>
   <si>
     <t>Sumida</t>
@@ -1333,10 +1321,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:MA50"/>
+  <dimension ref="A1:MA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5448,7 +5436,7 @@
         <v>96</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>97</v>
@@ -8816,16 +8804,16 @@
     <row r="21" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>40</v>
@@ -8834,11 +8822,9 @@
         <v>1932</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>148</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
         <v>89</v>
       </c>
@@ -8864,10 +8850,10 @@
         <v>105</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
@@ -9193,16 +9179,16 @@
     <row r="22" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>40</v>
@@ -9211,7 +9197,7 @@
         <v>1932</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
@@ -9239,11 +9225,9 @@
         <v>105</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>151</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -9568,16 +9552,16 @@
     <row r="23" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>40</v>
@@ -9586,7 +9570,7 @@
         <v>1932</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
@@ -9611,12 +9595,14 @@
         <v>45</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S23" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -9959,7 +9945,7 @@
         <v>1932</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
@@ -9984,13 +9970,13 @@
         <v>45</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
@@ -10316,16 +10302,16 @@
     <row r="25" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>40</v>
@@ -10334,7 +10320,7 @@
         <v>1932</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3" t="s">
@@ -10362,10 +10348,10 @@
         <v>90</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
@@ -10690,57 +10676,57 @@
     </row>
     <row r="26" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="8">
         <v>1932</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3" t="s">
+      <c r="I26" s="8"/>
+      <c r="J26" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="P26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="S26" s="3" t="s">
+      <c r="Q26" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="R26" s="8" t="s">
         <v>66</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
@@ -10751,23 +10737,55 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
+      <c r="AC26" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF26" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="AI26" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
-      <c r="AL26" s="3"/>
-      <c r="AM26" s="3"/>
-      <c r="AN26" s="3"/>
-      <c r="AO26" s="3"/>
-      <c r="AP26" s="3"/>
-      <c r="AQ26" s="3"/>
-      <c r="AR26" s="3"/>
-      <c r="AS26" s="3"/>
+      <c r="AK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR26" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS26" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="AT26" s="3"/>
       <c r="AU26" s="3"/>
       <c r="AV26" s="3"/>
@@ -10777,23 +10795,55 @@
       <c r="AZ26" s="3"/>
       <c r="BA26" s="3"/>
       <c r="BB26" s="3"/>
-      <c r="BC26" s="3"/>
-      <c r="BD26" s="3"/>
-      <c r="BE26" s="3"/>
-      <c r="BF26" s="3"/>
-      <c r="BG26" s="3"/>
-      <c r="BH26" s="3"/>
-      <c r="BI26" s="3"/>
+      <c r="BC26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD26" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="BE26" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="BF26" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="BI26" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="BJ26" s="3"/>
-      <c r="BK26" s="3"/>
-      <c r="BL26" s="3"/>
-      <c r="BM26" s="3"/>
-      <c r="BN26" s="3"/>
-      <c r="BO26" s="3"/>
-      <c r="BP26" s="3"/>
-      <c r="BQ26" s="3"/>
-      <c r="BR26" s="3"/>
-      <c r="BS26" s="3"/>
+      <c r="BK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="BM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="BQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BR26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BS26" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="BT26" s="3"/>
       <c r="BU26" s="3"/>
       <c r="BV26" s="3"/>
@@ -10803,24 +10853,58 @@
       <c r="BZ26" s="3"/>
       <c r="CA26" s="3"/>
       <c r="CB26" s="3"/>
-      <c r="CC26" s="3"/>
-      <c r="CD26" s="3"/>
-      <c r="CE26" s="3"/>
-      <c r="CF26" s="3"/>
-      <c r="CG26" s="3"/>
-      <c r="CH26" s="3"/>
-      <c r="CI26" s="3"/>
+      <c r="CC26" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CD26" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="CE26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="CF26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="CG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="CH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="CI26" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="CJ26" s="3"/>
-      <c r="CK26" s="3"/>
-      <c r="CL26" s="3"/>
-      <c r="CM26" s="3"/>
-      <c r="CN26" s="3"/>
-      <c r="CO26" s="3"/>
-      <c r="CP26" s="3"/>
-      <c r="CQ26" s="3"/>
-      <c r="CR26" s="3"/>
-      <c r="CS26" s="3"/>
-      <c r="CT26" s="3"/>
+      <c r="CK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="CL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="CM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="CN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="CO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="CP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="CQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="CR26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="CS26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="CT26" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="CU26" s="3"/>
       <c r="CV26" s="3"/>
       <c r="CW26" s="3"/>
@@ -10829,24 +10913,58 @@
       <c r="CZ26" s="3"/>
       <c r="DA26" s="3"/>
       <c r="DB26" s="3"/>
-      <c r="DC26" s="3"/>
-      <c r="DD26" s="3"/>
-      <c r="DE26" s="3"/>
-      <c r="DF26" s="3"/>
-      <c r="DG26" s="3"/>
-      <c r="DH26" s="3"/>
-      <c r="DI26" s="3"/>
+      <c r="DC26" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="DD26" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="DE26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="DF26" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="DG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="DH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="DI26" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="DJ26" s="3"/>
-      <c r="DK26" s="3"/>
-      <c r="DL26" s="3"/>
-      <c r="DM26" s="3"/>
-      <c r="DN26" s="3"/>
-      <c r="DO26" s="3"/>
-      <c r="DP26" s="3"/>
-      <c r="DQ26" s="3"/>
-      <c r="DR26" s="3"/>
-      <c r="DS26" s="3"/>
-      <c r="DT26" s="3"/>
+      <c r="DK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="DL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="DM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="DN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="DO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="DP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="DQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="DR26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="DS26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="DT26" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="DU26" s="3"/>
       <c r="DV26" s="3"/>
       <c r="DW26" s="3"/>
@@ -10855,23 +10973,55 @@
       <c r="DZ26" s="3"/>
       <c r="EA26" s="3"/>
       <c r="EB26" s="3"/>
-      <c r="EC26" s="3"/>
-      <c r="ED26" s="3"/>
-      <c r="EE26" s="3"/>
-      <c r="EF26" s="3"/>
-      <c r="EG26" s="3"/>
-      <c r="EH26" s="3"/>
-      <c r="EI26" s="3"/>
+      <c r="EC26" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="ED26" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="EE26" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="EF26" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="EG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="EH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="EI26" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="EJ26" s="3"/>
-      <c r="EK26" s="3"/>
-      <c r="EL26" s="3"/>
-      <c r="EM26" s="3"/>
-      <c r="EN26" s="3"/>
-      <c r="EO26" s="3"/>
-      <c r="EP26" s="3"/>
-      <c r="EQ26" s="3"/>
-      <c r="ER26" s="3"/>
-      <c r="ES26" s="3"/>
+      <c r="EK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="EL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="EM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="EN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="EO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="EP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="EQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="ER26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="ES26" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="ET26" s="3"/>
       <c r="EU26" s="3"/>
       <c r="EV26" s="3"/>
@@ -10881,23 +11031,55 @@
       <c r="EZ26" s="3"/>
       <c r="FA26" s="3"/>
       <c r="FB26" s="3"/>
-      <c r="FC26" s="3"/>
-      <c r="FD26" s="3"/>
-      <c r="FE26" s="3"/>
-      <c r="FF26" s="3"/>
-      <c r="FG26" s="3"/>
-      <c r="FH26" s="3"/>
-      <c r="FI26" s="3"/>
+      <c r="FC26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="FD26" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="FE26" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="FF26" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="FG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="FH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="FI26" s="3" t="s">
+        <v>205</v>
+      </c>
       <c r="FJ26" s="3"/>
-      <c r="FK26" s="3"/>
-      <c r="FL26" s="3"/>
-      <c r="FM26" s="3"/>
-      <c r="FN26" s="3"/>
-      <c r="FO26" s="3"/>
-      <c r="FP26" s="3"/>
-      <c r="FQ26" s="3"/>
-      <c r="FR26" s="3"/>
-      <c r="FS26" s="3"/>
+      <c r="FK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="FL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="FM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="FN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="FO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="FP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="FQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="FR26" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="FS26" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="FT26" s="3"/>
       <c r="FU26" s="3"/>
       <c r="FV26" s="3"/>
@@ -10907,23 +11089,55 @@
       <c r="FZ26" s="3"/>
       <c r="GA26" s="3"/>
       <c r="GB26" s="3"/>
-      <c r="GC26" s="3"/>
-      <c r="GD26" s="3"/>
-      <c r="GE26" s="3"/>
-      <c r="GF26" s="3"/>
-      <c r="GG26" s="3"/>
-      <c r="GH26" s="3"/>
-      <c r="GI26" s="3"/>
+      <c r="GC26" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="GD26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="GE26" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="GF26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="GG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="GH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="GI26" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="GJ26" s="3"/>
-      <c r="GK26" s="3"/>
-      <c r="GL26" s="3"/>
-      <c r="GM26" s="3"/>
-      <c r="GN26" s="3"/>
-      <c r="GO26" s="3"/>
-      <c r="GP26" s="3"/>
-      <c r="GQ26" s="3"/>
-      <c r="GR26" s="3"/>
-      <c r="GS26" s="3"/>
+      <c r="GK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="GL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="GM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="GN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="GO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="GP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="GQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="GR26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="GS26" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="GT26" s="3"/>
       <c r="GU26" s="3"/>
       <c r="GV26" s="3"/>
@@ -10933,23 +11147,55 @@
       <c r="GZ26" s="3"/>
       <c r="HA26" s="3"/>
       <c r="HB26" s="3"/>
-      <c r="HC26" s="3"/>
-      <c r="HD26" s="3"/>
-      <c r="HE26" s="3"/>
-      <c r="HF26" s="3"/>
-      <c r="HG26" s="3"/>
-      <c r="HH26" s="3"/>
-      <c r="HI26" s="3"/>
+      <c r="HC26" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="HD26" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="HE26" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="HF26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="HG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="HH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="HI26" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="HJ26" s="3"/>
-      <c r="HK26" s="3"/>
-      <c r="HL26" s="3"/>
-      <c r="HM26" s="3"/>
-      <c r="HN26" s="3"/>
-      <c r="HO26" s="3"/>
-      <c r="HP26" s="3"/>
-      <c r="HQ26" s="3"/>
-      <c r="HR26" s="3"/>
-      <c r="HS26" s="3"/>
+      <c r="HK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="HL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="HM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="HN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="HO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="HP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="HQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="HR26" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="HS26" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="HT26" s="3"/>
       <c r="HU26" s="3"/>
       <c r="HV26" s="3"/>
@@ -10959,22 +11205,52 @@
       <c r="HZ26" s="3"/>
       <c r="IA26" s="3"/>
       <c r="IB26" s="3"/>
-      <c r="IC26" s="3"/>
-      <c r="ID26" s="3"/>
-      <c r="IE26" s="3"/>
-      <c r="IF26" s="3"/>
-      <c r="IG26" s="3"/>
-      <c r="IH26" s="3"/>
-      <c r="II26" s="3"/>
+      <c r="IC26" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="ID26" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="IE26" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="IF26" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="IG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="IH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="II26" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="IJ26" s="3"/>
-      <c r="IK26" s="3"/>
-      <c r="IL26" s="3"/>
-      <c r="IM26" s="3"/>
-      <c r="IN26" s="3"/>
-      <c r="IO26" s="3"/>
-      <c r="IP26" s="3"/>
-      <c r="IQ26" s="3"/>
-      <c r="IR26" s="3"/>
+      <c r="IK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="IL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="IM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="IN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="IO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="IP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="IQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="IR26" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="IS26" s="3"/>
       <c r="IT26" s="3"/>
       <c r="IU26" s="3"/>
@@ -10985,22 +11261,52 @@
       <c r="IZ26" s="3"/>
       <c r="JA26" s="3"/>
       <c r="JB26" s="3"/>
-      <c r="JC26" s="3"/>
-      <c r="JD26" s="3"/>
-      <c r="JE26" s="3"/>
-      <c r="JF26" s="3"/>
-      <c r="JG26" s="3"/>
-      <c r="JH26" s="3"/>
-      <c r="JI26" s="3"/>
+      <c r="JC26" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="JD26" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="JE26" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="JF26" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="JG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="JH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="JI26" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="JJ26" s="3"/>
-      <c r="JK26" s="3"/>
-      <c r="JL26" s="3"/>
-      <c r="JM26" s="3"/>
-      <c r="JN26" s="3"/>
-      <c r="JO26" s="3"/>
-      <c r="JP26" s="3"/>
-      <c r="JQ26" s="3"/>
-      <c r="JR26" s="3"/>
+      <c r="JK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="JL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="JM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="JN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="JO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="JP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="JQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="JR26" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="JS26" s="3"/>
       <c r="JT26" s="3"/>
       <c r="JU26" s="3"/>
@@ -11011,23 +11317,57 @@
       <c r="JZ26" s="3"/>
       <c r="KA26" s="3"/>
       <c r="KB26" s="3"/>
-      <c r="KC26" s="3"/>
-      <c r="KD26" s="3"/>
-      <c r="KE26" s="3"/>
-      <c r="KF26" s="3"/>
-      <c r="KG26" s="3"/>
-      <c r="KH26" s="3"/>
-      <c r="KI26" s="3"/>
-      <c r="KJ26" s="3"/>
-      <c r="KK26" s="3"/>
-      <c r="KL26" s="3"/>
-      <c r="KM26" s="3"/>
-      <c r="KN26" s="3"/>
-      <c r="KO26" s="3"/>
-      <c r="KP26" s="3"/>
-      <c r="KQ26" s="3"/>
-      <c r="KR26" s="3"/>
-      <c r="KS26" s="3"/>
+      <c r="KC26" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="KD26" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="KE26" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="KF26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="KG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="KH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="KI26" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="KJ26" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="KK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="KL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="KM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="KN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="KO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="KP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="KQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="KR26" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="KS26" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="KT26" s="3"/>
       <c r="KU26" s="3"/>
       <c r="KV26" s="3"/>
@@ -11037,24 +11377,58 @@
       <c r="KZ26" s="3"/>
       <c r="LA26" s="3"/>
       <c r="LB26" s="3"/>
-      <c r="LC26" s="3"/>
-      <c r="LD26" s="3"/>
-      <c r="LE26" s="3"/>
-      <c r="LF26" s="3"/>
-      <c r="LG26" s="3"/>
-      <c r="LH26" s="3"/>
-      <c r="LI26" s="3"/>
+      <c r="LC26" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="LD26" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="LE26" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="LF26" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="LG26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="LH26" s="10">
+        <v>1932</v>
+      </c>
+      <c r="LI26" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="LJ26" s="3"/>
-      <c r="LK26" s="3"/>
-      <c r="LL26" s="3"/>
-      <c r="LM26" s="3"/>
-      <c r="LN26" s="3"/>
-      <c r="LO26" s="3"/>
-      <c r="LP26" s="3"/>
-      <c r="LQ26" s="3"/>
-      <c r="LR26" s="3"/>
-      <c r="LS26" s="3"/>
-      <c r="LT26" s="3"/>
+      <c r="LK26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="LL26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="LM26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="LN26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="LO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="LP26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="LQ26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="LR26" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="LS26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="LT26" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="LU26" s="3"/>
       <c r="LV26" s="3"/>
       <c r="LW26" s="3"/>
@@ -11066,16 +11440,16 @@
     <row r="27" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="8" t="s">
         <v>178</v>
       </c>
+      <c r="C27" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="E27" s="8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>40</v>
@@ -11083,10 +11457,10 @@
       <c r="G27" s="8">
         <v>1932</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I27" s="3"/>
       <c r="J27" s="8" t="s">
         <v>89</v>
       </c>
@@ -11109,14 +11483,12 @@
         <v>45</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="S27" s="9" t="s">
-        <v>181</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -11126,55 +11498,23 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
-      <c r="AC27" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AD27" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE27" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF27" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="AI27" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
-      <c r="AK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR27" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AS27" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
       <c r="AT27" s="3"/>
       <c r="AU27" s="3"/>
       <c r="AV27" s="3"/>
@@ -11184,55 +11524,23 @@
       <c r="AZ27" s="3"/>
       <c r="BA27" s="3"/>
       <c r="BB27" s="3"/>
-      <c r="BC27" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BD27" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BE27" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="BF27" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="BG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="BH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="BI27" s="3" t="s">
-        <v>191</v>
-      </c>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3"/>
+      <c r="BG27" s="3"/>
+      <c r="BH27" s="3"/>
+      <c r="BI27" s="3"/>
       <c r="BJ27" s="3"/>
-      <c r="BK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="BQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BR27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="BS27" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="BK27" s="3"/>
+      <c r="BL27" s="3"/>
+      <c r="BM27" s="3"/>
+      <c r="BN27" s="3"/>
+      <c r="BO27" s="3"/>
+      <c r="BP27" s="3"/>
+      <c r="BQ27" s="3"/>
+      <c r="BR27" s="3"/>
+      <c r="BS27" s="3"/>
       <c r="BT27" s="3"/>
       <c r="BU27" s="3"/>
       <c r="BV27" s="3"/>
@@ -11242,58 +11550,24 @@
       <c r="BZ27" s="3"/>
       <c r="CA27" s="3"/>
       <c r="CB27" s="3"/>
-      <c r="CC27" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CD27" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CE27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CF27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="CH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="CI27" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="CC27" s="3"/>
+      <c r="CD27" s="3"/>
+      <c r="CE27" s="3"/>
+      <c r="CF27" s="3"/>
+      <c r="CG27" s="3"/>
+      <c r="CH27" s="3"/>
+      <c r="CI27" s="3"/>
       <c r="CJ27" s="3"/>
-      <c r="CK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="CL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="CM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="CN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="CO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="CP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="CQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="CR27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="CS27" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="CT27" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="CK27" s="3"/>
+      <c r="CL27" s="3"/>
+      <c r="CM27" s="3"/>
+      <c r="CN27" s="3"/>
+      <c r="CO27" s="3"/>
+      <c r="CP27" s="3"/>
+      <c r="CQ27" s="3"/>
+      <c r="CR27" s="3"/>
+      <c r="CS27" s="3"/>
+      <c r="CT27" s="3"/>
       <c r="CU27" s="3"/>
       <c r="CV27" s="3"/>
       <c r="CW27" s="3"/>
@@ -11302,58 +11576,24 @@
       <c r="CZ27" s="3"/>
       <c r="DA27" s="3"/>
       <c r="DB27" s="3"/>
-      <c r="DC27" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="DD27" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="DE27" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="DF27" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="DG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="DH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="DI27" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="DC27" s="3"/>
+      <c r="DD27" s="3"/>
+      <c r="DE27" s="3"/>
+      <c r="DF27" s="3"/>
+      <c r="DG27" s="3"/>
+      <c r="DH27" s="3"/>
+      <c r="DI27" s="3"/>
       <c r="DJ27" s="3"/>
-      <c r="DK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="DL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="DM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="DN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="DO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="DP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="DQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="DR27" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="DS27" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="DT27" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="DK27" s="3"/>
+      <c r="DL27" s="3"/>
+      <c r="DM27" s="3"/>
+      <c r="DN27" s="3"/>
+      <c r="DO27" s="3"/>
+      <c r="DP27" s="3"/>
+      <c r="DQ27" s="3"/>
+      <c r="DR27" s="3"/>
+      <c r="DS27" s="3"/>
+      <c r="DT27" s="3"/>
       <c r="DU27" s="3"/>
       <c r="DV27" s="3"/>
       <c r="DW27" s="3"/>
@@ -11362,55 +11602,23 @@
       <c r="DZ27" s="3"/>
       <c r="EA27" s="3"/>
       <c r="EB27" s="3"/>
-      <c r="EC27" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="ED27" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="EE27" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="EF27" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="EG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="EH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="EI27" s="3" t="s">
-        <v>191</v>
-      </c>
+      <c r="EC27" s="3"/>
+      <c r="ED27" s="3"/>
+      <c r="EE27" s="3"/>
+      <c r="EF27" s="3"/>
+      <c r="EG27" s="3"/>
+      <c r="EH27" s="3"/>
+      <c r="EI27" s="3"/>
       <c r="EJ27" s="3"/>
-      <c r="EK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="EL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="EM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="EN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="EO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="EP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="EQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="ER27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="ES27" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="EK27" s="3"/>
+      <c r="EL27" s="3"/>
+      <c r="EM27" s="3"/>
+      <c r="EN27" s="3"/>
+      <c r="EO27" s="3"/>
+      <c r="EP27" s="3"/>
+      <c r="EQ27" s="3"/>
+      <c r="ER27" s="3"/>
+      <c r="ES27" s="3"/>
       <c r="ET27" s="3"/>
       <c r="EU27" s="3"/>
       <c r="EV27" s="3"/>
@@ -11420,55 +11628,23 @@
       <c r="EZ27" s="3"/>
       <c r="FA27" s="3"/>
       <c r="FB27" s="3"/>
-      <c r="FC27" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="FD27" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="FE27" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="FF27" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="FG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="FH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="FI27" s="3" t="s">
-        <v>209</v>
-      </c>
+      <c r="FC27" s="3"/>
+      <c r="FD27" s="3"/>
+      <c r="FE27" s="3"/>
+      <c r="FF27" s="3"/>
+      <c r="FG27" s="3"/>
+      <c r="FH27" s="3"/>
+      <c r="FI27" s="3"/>
       <c r="FJ27" s="3"/>
-      <c r="FK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="FL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="FM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="FN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="FO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="FP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="FQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="FR27" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="FS27" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="FK27" s="3"/>
+      <c r="FL27" s="3"/>
+      <c r="FM27" s="3"/>
+      <c r="FN27" s="3"/>
+      <c r="FO27" s="3"/>
+      <c r="FP27" s="3"/>
+      <c r="FQ27" s="3"/>
+      <c r="FR27" s="3"/>
+      <c r="FS27" s="3"/>
       <c r="FT27" s="3"/>
       <c r="FU27" s="3"/>
       <c r="FV27" s="3"/>
@@ -11478,55 +11654,23 @@
       <c r="FZ27" s="3"/>
       <c r="GA27" s="3"/>
       <c r="GB27" s="3"/>
-      <c r="GC27" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="GD27" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="GE27" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="GF27" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="GG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="GH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="GI27" s="3" t="s">
-        <v>214</v>
-      </c>
+      <c r="GC27" s="3"/>
+      <c r="GD27" s="3"/>
+      <c r="GE27" s="3"/>
+      <c r="GF27" s="3"/>
+      <c r="GG27" s="3"/>
+      <c r="GH27" s="3"/>
+      <c r="GI27" s="3"/>
       <c r="GJ27" s="3"/>
-      <c r="GK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="GL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="GM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="GN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="GO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="GP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="GQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="GR27" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="GS27" s="3" t="s">
-        <v>215</v>
-      </c>
+      <c r="GK27" s="3"/>
+      <c r="GL27" s="3"/>
+      <c r="GM27" s="3"/>
+      <c r="GN27" s="3"/>
+      <c r="GO27" s="3"/>
+      <c r="GP27" s="3"/>
+      <c r="GQ27" s="3"/>
+      <c r="GR27" s="3"/>
+      <c r="GS27" s="3"/>
       <c r="GT27" s="3"/>
       <c r="GU27" s="3"/>
       <c r="GV27" s="3"/>
@@ -11536,55 +11680,23 @@
       <c r="GZ27" s="3"/>
       <c r="HA27" s="3"/>
       <c r="HB27" s="3"/>
-      <c r="HC27" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="HD27" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="HE27" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="HF27" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="HG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="HH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="HI27" s="3" t="s">
-        <v>214</v>
-      </c>
+      <c r="HC27" s="3"/>
+      <c r="HD27" s="3"/>
+      <c r="HE27" s="3"/>
+      <c r="HF27" s="3"/>
+      <c r="HG27" s="3"/>
+      <c r="HH27" s="3"/>
+      <c r="HI27" s="3"/>
       <c r="HJ27" s="3"/>
-      <c r="HK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="HL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="HM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="HN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="HO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="HP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="HQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="HR27" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="HS27" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="HK27" s="3"/>
+      <c r="HL27" s="3"/>
+      <c r="HM27" s="3"/>
+      <c r="HN27" s="3"/>
+      <c r="HO27" s="3"/>
+      <c r="HP27" s="3"/>
+      <c r="HQ27" s="3"/>
+      <c r="HR27" s="3"/>
+      <c r="HS27" s="3"/>
       <c r="HT27" s="3"/>
       <c r="HU27" s="3"/>
       <c r="HV27" s="3"/>
@@ -11594,52 +11706,22 @@
       <c r="HZ27" s="3"/>
       <c r="IA27" s="3"/>
       <c r="IB27" s="3"/>
-      <c r="IC27" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="ID27" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="IE27" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="IF27" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="IG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="IH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="II27" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="IC27" s="3"/>
+      <c r="ID27" s="3"/>
+      <c r="IE27" s="3"/>
+      <c r="IF27" s="3"/>
+      <c r="IG27" s="3"/>
+      <c r="IH27" s="3"/>
+      <c r="II27" s="3"/>
       <c r="IJ27" s="3"/>
-      <c r="IK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="IL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="IM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="IN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="IO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="IP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="IQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="IR27" s="3" t="s">
-        <v>225</v>
-      </c>
+      <c r="IK27" s="3"/>
+      <c r="IL27" s="3"/>
+      <c r="IM27" s="3"/>
+      <c r="IN27" s="3"/>
+      <c r="IO27" s="3"/>
+      <c r="IP27" s="3"/>
+      <c r="IQ27" s="3"/>
+      <c r="IR27" s="3"/>
       <c r="IS27" s="3"/>
       <c r="IT27" s="3"/>
       <c r="IU27" s="3"/>
@@ -11650,52 +11732,22 @@
       <c r="IZ27" s="3"/>
       <c r="JA27" s="3"/>
       <c r="JB27" s="3"/>
-      <c r="JC27" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="JD27" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="JE27" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="JF27" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="JG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="JH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="JI27" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="JC27" s="3"/>
+      <c r="JD27" s="3"/>
+      <c r="JE27" s="3"/>
+      <c r="JF27" s="3"/>
+      <c r="JG27" s="3"/>
+      <c r="JH27" s="3"/>
+      <c r="JI27" s="3"/>
       <c r="JJ27" s="3"/>
-      <c r="JK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="JL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="JM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="JN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="JO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="JP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="JQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="JR27" s="3" t="s">
-        <v>225</v>
-      </c>
+      <c r="JK27" s="3"/>
+      <c r="JL27" s="3"/>
+      <c r="JM27" s="3"/>
+      <c r="JN27" s="3"/>
+      <c r="JO27" s="3"/>
+      <c r="JP27" s="3"/>
+      <c r="JQ27" s="3"/>
+      <c r="JR27" s="3"/>
       <c r="JS27" s="3"/>
       <c r="JT27" s="3"/>
       <c r="JU27" s="3"/>
@@ -11706,57 +11758,23 @@
       <c r="JZ27" s="3"/>
       <c r="KA27" s="3"/>
       <c r="KB27" s="3"/>
-      <c r="KC27" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="KD27" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="KE27" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="KF27" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="KG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="KH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="KI27" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="KJ27" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="KK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="KL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="KM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="KN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="KO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="KP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="KQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="KR27" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="KS27" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="KC27" s="3"/>
+      <c r="KD27" s="3"/>
+      <c r="KE27" s="3"/>
+      <c r="KF27" s="3"/>
+      <c r="KG27" s="3"/>
+      <c r="KH27" s="3"/>
+      <c r="KI27" s="3"/>
+      <c r="KJ27" s="3"/>
+      <c r="KK27" s="3"/>
+      <c r="KL27" s="3"/>
+      <c r="KM27" s="3"/>
+      <c r="KN27" s="3"/>
+      <c r="KO27" s="3"/>
+      <c r="KP27" s="3"/>
+      <c r="KQ27" s="3"/>
+      <c r="KR27" s="3"/>
+      <c r="KS27" s="3"/>
       <c r="KT27" s="3"/>
       <c r="KU27" s="3"/>
       <c r="KV27" s="3"/>
@@ -11766,58 +11784,24 @@
       <c r="KZ27" s="3"/>
       <c r="LA27" s="3"/>
       <c r="LB27" s="3"/>
-      <c r="LC27" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="LD27" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="LE27" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="LF27" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="LG27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="LH27" s="10">
-        <v>1932</v>
-      </c>
-      <c r="LI27" s="3" t="s">
-        <v>241</v>
-      </c>
+      <c r="LC27" s="3"/>
+      <c r="LD27" s="3"/>
+      <c r="LE27" s="3"/>
+      <c r="LF27" s="3"/>
+      <c r="LG27" s="3"/>
+      <c r="LH27" s="3"/>
+      <c r="LI27" s="3"/>
       <c r="LJ27" s="3"/>
-      <c r="LK27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="LL27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="LM27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="LN27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="LO27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="LP27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="LQ27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="LR27" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="LS27" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="LT27" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="LK27" s="3"/>
+      <c r="LL27" s="3"/>
+      <c r="LM27" s="3"/>
+      <c r="LN27" s="3"/>
+      <c r="LO27" s="3"/>
+      <c r="LP27" s="3"/>
+      <c r="LQ27" s="3"/>
+      <c r="LR27" s="3"/>
+      <c r="LS27" s="3"/>
+      <c r="LT27" s="3"/>
       <c r="LU27" s="3"/>
       <c r="LV27" s="3"/>
       <c r="LW27" s="3"/>
@@ -11829,16 +11813,16 @@
     <row r="28" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>40</v>
@@ -11847,7 +11831,7 @@
         <v>1932</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="8" t="s">
@@ -11872,10 +11856,10 @@
         <v>45</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>145</v>
+        <v>64</v>
       </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -12202,15 +12186,15 @@
     <row r="29" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E29" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>190</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -12220,7 +12204,7 @@
         <v>1932</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="8" t="s">
@@ -12245,12 +12229,14 @@
         <v>45</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="R29" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="S29" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
@@ -12583,8 +12569,8 @@
       <c r="D30" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>194</v>
+      <c r="E30" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>40</v>
@@ -12593,7 +12579,7 @@
         <v>1932</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="8" t="s">
@@ -12618,13 +12604,13 @@
         <v>45</v>
       </c>
       <c r="Q30" s="8" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="R30" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="S30" s="8" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
@@ -12950,16 +12936,16 @@
     <row r="31" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>40</v>
@@ -12968,7 +12954,7 @@
         <v>1932</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="8" t="s">
@@ -12993,14 +12979,12 @@
         <v>45</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>175</v>
+        <v>66</v>
       </c>
       <c r="R31" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="S31" s="8" t="s">
-        <v>145</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
@@ -13343,7 +13327,7 @@
         <v>1932</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="8" t="s">
@@ -13368,10 +13352,10 @@
         <v>45</v>
       </c>
       <c r="Q32" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="R32" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="R32" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -13698,16 +13682,16 @@
     <row r="33" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="9" t="s">
         <v>207</v>
       </c>
+      <c r="D33" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="E33" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>40</v>
@@ -13716,7 +13700,7 @@
         <v>1932</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="8" t="s">
@@ -13741,10 +13725,10 @@
         <v>45</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -14071,16 +14055,16 @@
     <row r="34" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>40</v>
@@ -14089,7 +14073,7 @@
         <v>1932</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="8" t="s">
@@ -14114,10 +14098,10 @@
         <v>45</v>
       </c>
       <c r="Q34" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="R34" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="R34" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -14444,16 +14428,16 @@
     <row r="35" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>40</v>
@@ -14462,7 +14446,7 @@
         <v>1932</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>214</v>
+        <v>138</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="8" t="s">
@@ -14486,12 +14470,10 @@
       <c r="P35" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q35" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="R35" s="8" t="s">
-        <v>132</v>
-      </c>
+      <c r="Q35" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
@@ -14817,16 +14799,16 @@
     <row r="36" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>40</v>
@@ -14835,7 +14817,7 @@
         <v>1932</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="8" t="s">
@@ -14860,7 +14842,7 @@
         <v>45</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
@@ -15206,9 +15188,11 @@
         <v>1932</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I37" s="3"/>
+        <v>230</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="J37" s="8" t="s">
         <v>89</v>
       </c>
@@ -15230,10 +15214,12 @@
       <c r="P37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q37" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="R37" s="3"/>
+      <c r="Q37" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
@@ -15559,16 +15545,16 @@
     <row r="38" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>40</v>
@@ -15577,11 +15563,9 @@
         <v>1932</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>235</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="I38" s="3"/>
       <c r="J38" s="8" t="s">
         <v>89</v>
       </c>
@@ -15604,12 +15588,14 @@
         <v>45</v>
       </c>
       <c r="Q38" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="R38" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="S38" s="3"/>
+        <v>239</v>
+      </c>
+      <c r="S38" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -15933,63 +15919,61 @@
     </row>
     <row r="39" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
-      <c r="B39" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="B39" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="C39" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="11">
         <v>1932</v>
       </c>
-      <c r="H39" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="8" t="s">
+      <c r="H39" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M39" s="8" t="s">
+      <c r="M39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="N39" s="8" t="s">
+      <c r="N39" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="O39" s="8" t="s">
+      <c r="O39" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="P39" s="8" t="s">
+      <c r="P39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="Q39" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="R39" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="S39" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
+      <c r="Q39" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="R39" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
@@ -16309,16 +16293,16 @@
     <row r="40" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>40</v>
@@ -16327,7 +16311,7 @@
         <v>1932</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I40" s="11"/>
       <c r="J40" s="11" t="s">
@@ -16352,12 +16336,14 @@
         <v>45</v>
       </c>
       <c r="Q40" s="11" t="s">
-        <v>156</v>
+        <v>250</v>
       </c>
       <c r="R40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="S40" s="11"/>
+        <v>251</v>
+      </c>
+      <c r="S40" s="11" t="s">
+        <v>145</v>
+      </c>
       <c r="T40" s="11"/>
       <c r="U40" s="11"/>
       <c r="V40" s="11"/>
@@ -16682,16 +16668,16 @@
     <row r="41" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="11" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>40</v>
@@ -16700,7 +16686,7 @@
         <v>1932</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>253</v>
+        <v>104</v>
       </c>
       <c r="I41" s="11"/>
       <c r="J41" s="11" t="s">
@@ -16725,15 +16711,17 @@
         <v>45</v>
       </c>
       <c r="Q41" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="R41" s="11" t="s">
-        <v>255</v>
+        <v>152</v>
       </c>
       <c r="S41" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="T41" s="11"/>
+        <v>256</v>
+      </c>
+      <c r="T41" s="11" t="s">
+        <v>238</v>
+      </c>
       <c r="U41" s="11"/>
       <c r="V41" s="11"/>
       <c r="W41" s="11"/>
@@ -17057,16 +17045,16 @@
     <row r="42" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>40</v>
@@ -17075,7 +17063,7 @@
         <v>1932</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>104</v>
+        <v>261</v>
       </c>
       <c r="I42" s="11"/>
       <c r="J42" s="11" t="s">
@@ -17100,17 +17088,15 @@
         <v>45</v>
       </c>
       <c r="Q42" s="11" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="R42" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="S42" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="T42" s="11" t="s">
-        <v>242</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="T42" s="11"/>
       <c r="U42" s="11"/>
       <c r="V42" s="11"/>
       <c r="W42" s="11"/>
@@ -17434,16 +17420,16 @@
     <row r="43" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>40</v>
@@ -17452,7 +17438,7 @@
         <v>1932</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>265</v>
+        <v>77</v>
       </c>
       <c r="I43" s="11"/>
       <c r="J43" s="11" t="s">
@@ -17477,13 +17463,13 @@
         <v>45</v>
       </c>
       <c r="Q43" s="11" t="s">
-        <v>266</v>
+        <v>152</v>
       </c>
       <c r="R43" s="11" t="s">
-        <v>156</v>
+        <v>267</v>
       </c>
       <c r="S43" s="11" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="T43" s="11"/>
       <c r="U43" s="11"/>
@@ -17809,16 +17795,16 @@
     <row r="44" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>40</v>
@@ -17827,7 +17813,7 @@
         <v>1932</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="I44" s="11"/>
       <c r="J44" s="11" t="s">
@@ -17852,15 +17838,17 @@
         <v>45</v>
       </c>
       <c r="Q44" s="11" t="s">
-        <v>156</v>
+        <v>64</v>
       </c>
       <c r="R44" s="11" t="s">
-        <v>271</v>
+        <v>72</v>
       </c>
       <c r="S44" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="T44" s="11"/>
+      <c r="T44" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="U44" s="11"/>
       <c r="V44" s="11"/>
       <c r="W44" s="11"/>
@@ -18184,16 +18172,16 @@
     <row r="45" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>40</v>
@@ -18202,9 +18190,11 @@
         <v>1932</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="I45" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="J45" s="11" t="s">
         <v>89</v>
       </c>
@@ -18227,17 +18217,11 @@
         <v>45</v>
       </c>
       <c r="Q45" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="R45" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="S45" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="T45" s="11" t="s">
-        <v>63</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
       <c r="U45" s="11"/>
       <c r="V45" s="11"/>
       <c r="W45" s="11"/>
@@ -18561,16 +18545,16 @@
     <row r="46" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>40</v>
@@ -18579,11 +18563,9 @@
         <v>1932</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>95</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="I46" s="11"/>
       <c r="J46" s="11" t="s">
         <v>89</v>
       </c>
@@ -18606,7 +18588,7 @@
         <v>45</v>
       </c>
       <c r="Q46" s="11" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="R46" s="11"/>
       <c r="S46" s="11"/>
@@ -18934,16 +18916,16 @@
     <row r="47" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>40</v>
@@ -18952,7 +18934,7 @@
         <v>1932</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>286</v>
+        <v>61</v>
       </c>
       <c r="I47" s="11"/>
       <c r="J47" s="11" t="s">
@@ -18977,9 +18959,11 @@
         <v>45</v>
       </c>
       <c r="Q47" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="R47" s="11"/>
+        <v>177</v>
+      </c>
+      <c r="R47" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="S47" s="11"/>
       <c r="T47" s="11"/>
       <c r="U47" s="11"/>
@@ -19323,7 +19307,7 @@
         <v>1932</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>61</v>
+        <v>291</v>
       </c>
       <c r="I48" s="11"/>
       <c r="J48" s="11" t="s">
@@ -19348,10 +19332,10 @@
         <v>45</v>
       </c>
       <c r="Q48" s="11" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="R48" s="11" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="S48" s="11"/>
       <c r="T48" s="11"/>
@@ -19678,16 +19662,16 @@
     <row r="49" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="B49" s="11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>40</v>
@@ -19695,9 +19679,7 @@
       <c r="G49" s="11">
         <v>1932</v>
       </c>
-      <c r="H49" s="11" t="s">
-        <v>295</v>
-      </c>
+      <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11" t="s">
         <v>89</v>
@@ -19721,11 +19703,9 @@
         <v>45</v>
       </c>
       <c r="Q49" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="R49" s="11" t="s">
-        <v>133</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="R49" s="11"/>
       <c r="S49" s="11"/>
       <c r="T49" s="11"/>
       <c r="U49" s="11"/>
@@ -20048,375 +20028,6 @@
       <c r="LZ49" s="3"/>
       <c r="MA49" s="3"/>
     </row>
-    <row r="50" spans="1:339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="3"/>
-      <c r="B50" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G50" s="11">
-        <v>1932</v>
-      </c>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="L50" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="M50" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N50" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O50" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="P50" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q50" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AA50" s="3"/>
-      <c r="AB50" s="3"/>
-      <c r="AC50" s="3"/>
-      <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
-      <c r="AF50" s="3"/>
-      <c r="AG50" s="3"/>
-      <c r="AH50" s="3"/>
-      <c r="AI50" s="3"/>
-      <c r="AJ50" s="3"/>
-      <c r="AK50" s="3"/>
-      <c r="AL50" s="3"/>
-      <c r="AM50" s="3"/>
-      <c r="AN50" s="3"/>
-      <c r="AO50" s="3"/>
-      <c r="AP50" s="3"/>
-      <c r="AQ50" s="3"/>
-      <c r="AR50" s="3"/>
-      <c r="AS50" s="3"/>
-      <c r="AT50" s="3"/>
-      <c r="AU50" s="3"/>
-      <c r="AV50" s="3"/>
-      <c r="AW50" s="3"/>
-      <c r="AX50" s="3"/>
-      <c r="AY50" s="3"/>
-      <c r="AZ50" s="3"/>
-      <c r="BA50" s="3"/>
-      <c r="BB50" s="3"/>
-      <c r="BC50" s="3"/>
-      <c r="BD50" s="3"/>
-      <c r="BE50" s="3"/>
-      <c r="BF50" s="3"/>
-      <c r="BG50" s="3"/>
-      <c r="BH50" s="3"/>
-      <c r="BI50" s="3"/>
-      <c r="BJ50" s="3"/>
-      <c r="BK50" s="3"/>
-      <c r="BL50" s="3"/>
-      <c r="BM50" s="3"/>
-      <c r="BN50" s="3"/>
-      <c r="BO50" s="3"/>
-      <c r="BP50" s="3"/>
-      <c r="BQ50" s="3"/>
-      <c r="BR50" s="3"/>
-      <c r="BS50" s="3"/>
-      <c r="BT50" s="3"/>
-      <c r="BU50" s="3"/>
-      <c r="BV50" s="3"/>
-      <c r="BW50" s="3"/>
-      <c r="BX50" s="3"/>
-      <c r="BY50" s="3"/>
-      <c r="BZ50" s="3"/>
-      <c r="CA50" s="3"/>
-      <c r="CB50" s="3"/>
-      <c r="CC50" s="3"/>
-      <c r="CD50" s="3"/>
-      <c r="CE50" s="3"/>
-      <c r="CF50" s="3"/>
-      <c r="CG50" s="3"/>
-      <c r="CH50" s="3"/>
-      <c r="CI50" s="3"/>
-      <c r="CJ50" s="3"/>
-      <c r="CK50" s="3"/>
-      <c r="CL50" s="3"/>
-      <c r="CM50" s="3"/>
-      <c r="CN50" s="3"/>
-      <c r="CO50" s="3"/>
-      <c r="CP50" s="3"/>
-      <c r="CQ50" s="3"/>
-      <c r="CR50" s="3"/>
-      <c r="CS50" s="3"/>
-      <c r="CT50" s="3"/>
-      <c r="CU50" s="3"/>
-      <c r="CV50" s="3"/>
-      <c r="CW50" s="3"/>
-      <c r="CX50" s="3"/>
-      <c r="CY50" s="3"/>
-      <c r="CZ50" s="3"/>
-      <c r="DA50" s="3"/>
-      <c r="DB50" s="3"/>
-      <c r="DC50" s="3"/>
-      <c r="DD50" s="3"/>
-      <c r="DE50" s="3"/>
-      <c r="DF50" s="3"/>
-      <c r="DG50" s="3"/>
-      <c r="DH50" s="3"/>
-      <c r="DI50" s="3"/>
-      <c r="DJ50" s="3"/>
-      <c r="DK50" s="3"/>
-      <c r="DL50" s="3"/>
-      <c r="DM50" s="3"/>
-      <c r="DN50" s="3"/>
-      <c r="DO50" s="3"/>
-      <c r="DP50" s="3"/>
-      <c r="DQ50" s="3"/>
-      <c r="DR50" s="3"/>
-      <c r="DS50" s="3"/>
-      <c r="DT50" s="3"/>
-      <c r="DU50" s="3"/>
-      <c r="DV50" s="3"/>
-      <c r="DW50" s="3"/>
-      <c r="DX50" s="3"/>
-      <c r="DY50" s="3"/>
-      <c r="DZ50" s="3"/>
-      <c r="EA50" s="3"/>
-      <c r="EB50" s="3"/>
-      <c r="EC50" s="3"/>
-      <c r="ED50" s="3"/>
-      <c r="EE50" s="3"/>
-      <c r="EF50" s="3"/>
-      <c r="EG50" s="3"/>
-      <c r="EH50" s="3"/>
-      <c r="EI50" s="3"/>
-      <c r="EJ50" s="3"/>
-      <c r="EK50" s="3"/>
-      <c r="EL50" s="3"/>
-      <c r="EM50" s="3"/>
-      <c r="EN50" s="3"/>
-      <c r="EO50" s="3"/>
-      <c r="EP50" s="3"/>
-      <c r="EQ50" s="3"/>
-      <c r="ER50" s="3"/>
-      <c r="ES50" s="3"/>
-      <c r="ET50" s="3"/>
-      <c r="EU50" s="3"/>
-      <c r="EV50" s="3"/>
-      <c r="EW50" s="3"/>
-      <c r="EX50" s="3"/>
-      <c r="EY50" s="3"/>
-      <c r="EZ50" s="3"/>
-      <c r="FA50" s="3"/>
-      <c r="FB50" s="3"/>
-      <c r="FC50" s="3"/>
-      <c r="FD50" s="3"/>
-      <c r="FE50" s="3"/>
-      <c r="FF50" s="3"/>
-      <c r="FG50" s="3"/>
-      <c r="FH50" s="3"/>
-      <c r="FI50" s="3"/>
-      <c r="FJ50" s="3"/>
-      <c r="FK50" s="3"/>
-      <c r="FL50" s="3"/>
-      <c r="FM50" s="3"/>
-      <c r="FN50" s="3"/>
-      <c r="FO50" s="3"/>
-      <c r="FP50" s="3"/>
-      <c r="FQ50" s="3"/>
-      <c r="FR50" s="3"/>
-      <c r="FS50" s="3"/>
-      <c r="FT50" s="3"/>
-      <c r="FU50" s="3"/>
-      <c r="FV50" s="3"/>
-      <c r="FW50" s="3"/>
-      <c r="FX50" s="3"/>
-      <c r="FY50" s="3"/>
-      <c r="FZ50" s="3"/>
-      <c r="GA50" s="3"/>
-      <c r="GB50" s="3"/>
-      <c r="GC50" s="3"/>
-      <c r="GD50" s="3"/>
-      <c r="GE50" s="3"/>
-      <c r="GF50" s="3"/>
-      <c r="GG50" s="3"/>
-      <c r="GH50" s="3"/>
-      <c r="GI50" s="3"/>
-      <c r="GJ50" s="3"/>
-      <c r="GK50" s="3"/>
-      <c r="GL50" s="3"/>
-      <c r="GM50" s="3"/>
-      <c r="GN50" s="3"/>
-      <c r="GO50" s="3"/>
-      <c r="GP50" s="3"/>
-      <c r="GQ50" s="3"/>
-      <c r="GR50" s="3"/>
-      <c r="GS50" s="3"/>
-      <c r="GT50" s="3"/>
-      <c r="GU50" s="3"/>
-      <c r="GV50" s="3"/>
-      <c r="GW50" s="3"/>
-      <c r="GX50" s="3"/>
-      <c r="GY50" s="3"/>
-      <c r="GZ50" s="3"/>
-      <c r="HA50" s="3"/>
-      <c r="HB50" s="3"/>
-      <c r="HC50" s="3"/>
-      <c r="HD50" s="3"/>
-      <c r="HE50" s="3"/>
-      <c r="HF50" s="3"/>
-      <c r="HG50" s="3"/>
-      <c r="HH50" s="3"/>
-      <c r="HI50" s="3"/>
-      <c r="HJ50" s="3"/>
-      <c r="HK50" s="3"/>
-      <c r="HL50" s="3"/>
-      <c r="HM50" s="3"/>
-      <c r="HN50" s="3"/>
-      <c r="HO50" s="3"/>
-      <c r="HP50" s="3"/>
-      <c r="HQ50" s="3"/>
-      <c r="HR50" s="3"/>
-      <c r="HS50" s="3"/>
-      <c r="HT50" s="3"/>
-      <c r="HU50" s="3"/>
-      <c r="HV50" s="3"/>
-      <c r="HW50" s="3"/>
-      <c r="HX50" s="3"/>
-      <c r="HY50" s="3"/>
-      <c r="HZ50" s="3"/>
-      <c r="IA50" s="3"/>
-      <c r="IB50" s="3"/>
-      <c r="IC50" s="3"/>
-      <c r="ID50" s="3"/>
-      <c r="IE50" s="3"/>
-      <c r="IF50" s="3"/>
-      <c r="IG50" s="3"/>
-      <c r="IH50" s="3"/>
-      <c r="II50" s="3"/>
-      <c r="IJ50" s="3"/>
-      <c r="IK50" s="3"/>
-      <c r="IL50" s="3"/>
-      <c r="IM50" s="3"/>
-      <c r="IN50" s="3"/>
-      <c r="IO50" s="3"/>
-      <c r="IP50" s="3"/>
-      <c r="IQ50" s="3"/>
-      <c r="IR50" s="3"/>
-      <c r="IS50" s="3"/>
-      <c r="IT50" s="3"/>
-      <c r="IU50" s="3"/>
-      <c r="IV50" s="3"/>
-      <c r="IW50" s="3"/>
-      <c r="IX50" s="3"/>
-      <c r="IY50" s="3"/>
-      <c r="IZ50" s="3"/>
-      <c r="JA50" s="3"/>
-      <c r="JB50" s="3"/>
-      <c r="JC50" s="3"/>
-      <c r="JD50" s="3"/>
-      <c r="JE50" s="3"/>
-      <c r="JF50" s="3"/>
-      <c r="JG50" s="3"/>
-      <c r="JH50" s="3"/>
-      <c r="JI50" s="3"/>
-      <c r="JJ50" s="3"/>
-      <c r="JK50" s="3"/>
-      <c r="JL50" s="3"/>
-      <c r="JM50" s="3"/>
-      <c r="JN50" s="3"/>
-      <c r="JO50" s="3"/>
-      <c r="JP50" s="3"/>
-      <c r="JQ50" s="3"/>
-      <c r="JR50" s="3"/>
-      <c r="JS50" s="3"/>
-      <c r="JT50" s="3"/>
-      <c r="JU50" s="3"/>
-      <c r="JV50" s="3"/>
-      <c r="JW50" s="3"/>
-      <c r="JX50" s="3"/>
-      <c r="JY50" s="3"/>
-      <c r="JZ50" s="3"/>
-      <c r="KA50" s="3"/>
-      <c r="KB50" s="3"/>
-      <c r="KC50" s="3"/>
-      <c r="KD50" s="3"/>
-      <c r="KE50" s="3"/>
-      <c r="KF50" s="3"/>
-      <c r="KG50" s="3"/>
-      <c r="KH50" s="3"/>
-      <c r="KI50" s="3"/>
-      <c r="KJ50" s="3"/>
-      <c r="KK50" s="3"/>
-      <c r="KL50" s="3"/>
-      <c r="KM50" s="3"/>
-      <c r="KN50" s="3"/>
-      <c r="KO50" s="3"/>
-      <c r="KP50" s="3"/>
-      <c r="KQ50" s="3"/>
-      <c r="KR50" s="3"/>
-      <c r="KS50" s="3"/>
-      <c r="KT50" s="3"/>
-      <c r="KU50" s="3"/>
-      <c r="KV50" s="3"/>
-      <c r="KW50" s="3"/>
-      <c r="KX50" s="3"/>
-      <c r="KY50" s="3"/>
-      <c r="KZ50" s="3"/>
-      <c r="LA50" s="3"/>
-      <c r="LB50" s="3"/>
-      <c r="LC50" s="3"/>
-      <c r="LD50" s="3"/>
-      <c r="LE50" s="3"/>
-      <c r="LF50" s="3"/>
-      <c r="LG50" s="3"/>
-      <c r="LH50" s="3"/>
-      <c r="LI50" s="3"/>
-      <c r="LJ50" s="3"/>
-      <c r="LK50" s="3"/>
-      <c r="LL50" s="3"/>
-      <c r="LM50" s="3"/>
-      <c r="LN50" s="3"/>
-      <c r="LO50" s="3"/>
-      <c r="LP50" s="3"/>
-      <c r="LQ50" s="3"/>
-      <c r="LR50" s="3"/>
-      <c r="LS50" s="3"/>
-      <c r="LT50" s="3"/>
-      <c r="LU50" s="3"/>
-      <c r="LV50" s="3"/>
-      <c r="LW50" s="3"/>
-      <c r="LX50" s="3"/>
-      <c r="LY50" s="3"/>
-      <c r="LZ50" s="3"/>
-      <c r="MA50" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E2:F2"/>

</xml_diff>